<commit_message>
update schema to reflect requests
update schema to reflect requests
</commit_message>
<xml_diff>
--- a/ics499_project_visual_bom_schema.xlsx
+++ b/ics499_project_visual_bom_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr updateLinks="never" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp7371\htdocs\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{14C152CC-D300-4F70-A9EB-94FD75CA7EE5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27568754-15E2-445F-A881-55AFFDE5D640}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{890048CD-57CD-472A-B7B8-1AD7617F7D03}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{890048CD-57CD-472A-B7B8-1AD7617F7D03}"/>
   </bookViews>
   <sheets>
     <sheet name="A2, A3, A4" sheetId="5" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="162">
   <si>
     <t>Completed</t>
   </si>
@@ -367,9 +367,6 @@
     <t>notes</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>Public Domain. No Support</t>
   </si>
   <si>
@@ -506,6 +503,33 @@
   </si>
   <si>
     <t>In the final project, you will build an application called "Visual BOM".</t>
+  </si>
+  <si>
+    <t>request_id</t>
+  </si>
+  <si>
+    <t>request_status</t>
+  </si>
+  <si>
+    <t>request_step</t>
+  </si>
+  <si>
+    <t>request_date</t>
+  </si>
+  <si>
+    <t>VARCHAR(30)</t>
+  </si>
+  <si>
+    <t>PQR_839_R1, XYZ_789_R2</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>Review Step, Inspection Step, Approval Step</t>
+  </si>
+  <si>
+    <t>Approved, Pending, Submitted</t>
   </si>
 </sst>
 </file>
@@ -516,7 +540,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -540,13 +564,25 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -561,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -577,6 +613,11 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -923,7 +964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70DBEC35-031D-4CC6-910F-AE25A8F437DD}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -931,17 +972,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -967,42 +1008,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1817,55 +1858,79 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838D4BE9-30EC-478D-A9EF-E4168FCD587C}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
     <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.77734375" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>105</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>104</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>100</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>98</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>96</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>94</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K1" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="O1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1879,24 +1944,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1913,7 +1978,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -1930,7 +1995,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>104</v>
       </c>
@@ -1947,7 +2012,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>102</v>
       </c>
@@ -1964,7 +2029,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>100</v>
       </c>
@@ -1981,7 +2046,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -1998,7 +2063,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -2015,7 +2080,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -2032,7 +2097,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -2050,28 +2115,93 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C21" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:I1">
+  <conditionalFormatting sqref="E1:O1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2109,7 +2239,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -2150,7 +2280,7 @@
         <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2">
         <v>1.1000000000000001</v>
@@ -2159,19 +2289,19 @@
         <v>101.1</v>
       </c>
       <c r="F2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G2">
         <v>2.2999999999999998</v>
       </c>
       <c r="H2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2182,7 +2312,7 @@
         <v>101</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3">
         <v>1.1000000000000001</v>
@@ -2191,22 +2321,22 @@
         <v>101.2</v>
       </c>
       <c r="F3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G3">
         <v>4.3</v>
       </c>
       <c r="H3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J3" t="s">
         <v>122</v>
       </c>
-      <c r="J3" t="s">
-        <v>123</v>
-      </c>
       <c r="K3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -2217,7 +2347,7 @@
         <v>101</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4">
         <v>1.1000000000000001</v>
@@ -2226,19 +2356,19 @@
         <v>101.3</v>
       </c>
       <c r="F4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -2249,7 +2379,7 @@
         <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5">
         <v>1.1000000000000001</v>
@@ -2258,19 +2388,19 @@
         <v>101.4</v>
       </c>
       <c r="F5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G5">
         <v>2019</v>
       </c>
       <c r="H5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" t="s">
         <v>121</v>
       </c>
-      <c r="I5" t="s">
-        <v>122</v>
-      </c>
       <c r="J5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -2281,7 +2411,7 @@
         <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D6">
         <v>1.1000000000000001</v>
@@ -2290,19 +2420,19 @@
         <v>101.5</v>
       </c>
       <c r="F6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G6">
         <v>2019</v>
       </c>
       <c r="H6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" t="s">
         <v>121</v>
       </c>
-      <c r="I6" t="s">
-        <v>122</v>
-      </c>
       <c r="J6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -2313,28 +2443,28 @@
         <v>101.1</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D7">
         <v>2.2999999999999998</v>
       </c>
       <c r="E7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" t="s">
         <v>128</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>129</v>
       </c>
-      <c r="G7" t="s">
-        <v>130</v>
-      </c>
       <c r="H7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -2345,28 +2475,28 @@
         <v>101.1</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D8">
         <v>2.2999999999999998</v>
       </c>
       <c r="E8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -2377,28 +2507,28 @@
         <v>101.1</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D9">
         <v>2.2999999999999998</v>
       </c>
       <c r="E9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -2409,7 +2539,7 @@
         <v>202</v>
       </c>
       <c r="C10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D10">
         <v>2.2000000000000002</v>
@@ -2418,19 +2548,19 @@
         <v>202.2</v>
       </c>
       <c r="F10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G10">
         <v>2.2999999999999998</v>
       </c>
       <c r="H10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2441,7 +2571,7 @@
         <v>202</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D11">
         <v>2.2000000000000002</v>
@@ -2450,22 +2580,22 @@
         <v>202.2</v>
       </c>
       <c r="F11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G11">
         <v>4.3</v>
       </c>
       <c r="H11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I11" t="s">
+        <v>121</v>
+      </c>
+      <c r="J11" t="s">
         <v>122</v>
       </c>
-      <c r="J11" t="s">
-        <v>123</v>
-      </c>
       <c r="K11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -2476,7 +2606,7 @@
         <v>202</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D12">
         <v>2.2000000000000002</v>
@@ -2485,19 +2615,19 @@
         <v>202.3</v>
       </c>
       <c r="F12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2508,7 +2638,7 @@
         <v>202</v>
       </c>
       <c r="C13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D13">
         <v>2.2000000000000002</v>
@@ -2517,19 +2647,19 @@
         <v>202.4</v>
       </c>
       <c r="F13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G13">
         <v>2029</v>
       </c>
       <c r="H13" t="s">
+        <v>120</v>
+      </c>
+      <c r="I13" t="s">
         <v>121</v>
       </c>
-      <c r="I13" t="s">
-        <v>122</v>
-      </c>
       <c r="J13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -2540,7 +2670,7 @@
         <v>202</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D14">
         <v>2.2000000000000002</v>
@@ -2549,19 +2679,19 @@
         <v>202.5</v>
       </c>
       <c r="F14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G14">
         <v>2029</v>
       </c>
       <c r="H14" t="s">
+        <v>120</v>
+      </c>
+      <c r="I14" t="s">
         <v>121</v>
       </c>
-      <c r="I14" t="s">
-        <v>122</v>
-      </c>
       <c r="J14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2572,28 +2702,28 @@
         <v>202.2</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D15">
         <v>2.2999999999999998</v>
       </c>
       <c r="E15" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" t="s">
+        <v>139</v>
+      </c>
+      <c r="G15" t="s">
         <v>136</v>
       </c>
-      <c r="F15" t="s">
-        <v>140</v>
-      </c>
-      <c r="G15" t="s">
-        <v>137</v>
-      </c>
       <c r="H15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2604,28 +2734,28 @@
         <v>202.2</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D16">
         <v>2.2999999999999998</v>
       </c>
       <c r="E16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F16" t="s">
+        <v>132</v>
+      </c>
+      <c r="G16" t="s">
         <v>136</v>
       </c>
-      <c r="F16" t="s">
-        <v>133</v>
-      </c>
-      <c r="G16" t="s">
-        <v>137</v>
-      </c>
       <c r="H16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2636,28 +2766,28 @@
         <v>202.2</v>
       </c>
       <c r="C17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D17">
         <v>2.2999999999999998</v>
       </c>
       <c r="E17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -2668,28 +2798,28 @@
         <v>202.2</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D18">
         <v>2.2999999999999998</v>
       </c>
       <c r="E18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2700,28 +2830,28 @@
         <v>202.2</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D19">
         <v>2.2999999999999998</v>
       </c>
       <c r="E19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19" t="s">
         <v>141</v>
       </c>
-      <c r="F19" t="s">
-        <v>142</v>
-      </c>
       <c r="G19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>